<commit_message>
update tc4 tc ly
</commit_message>
<xml_diff>
--- a/MiddleAssignment_LeTuanSang/TestCase4/TestCase4_LeTuanSang.xlsx
+++ b/MiddleAssignment_LeTuanSang/TestCase4/TestCase4_LeTuanSang.xlsx
@@ -455,7 +455,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="409">
   <si>
     <r>
       <rPr>
@@ -1879,32 +1879,6 @@
 4. Observe Full name</t>
   </si>
   <si>
-    <t xml:space="preserve">4. Address is saved successfully and displayed on the top of Address Book
-</t>
-  </si>
-  <si>
-    <t>1. Input Full name "CREATE DATABASE 1" 
-2. Input valid data on all mandatory fields
-3. Click on Save button
-4. Observe Full name</t>
-  </si>
-  <si>
-    <t>1. Paste valid data on Full name 
-2. Input valid data on all mandatory fields
-3. Click on Save button
-4. Observe Full name</t>
-  </si>
-  <si>
-    <t>1. Input valid data on Full name and all mandatory fields
-2. Click on X icon
-3. Click on Save button
-4. Observe Full name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.1 Address is NOT saved successfully
-4.2 Show error message below the Full Name field: "Please enter your Full name" </t>
-  </si>
-  <si>
     <t>1. Input Full name 1 Alphanumeric 
 2. Input valid data on all mandatory fields
 3. Click on Save button
@@ -1981,16 +1955,44 @@
 abcyxz</t>
   </si>
   <si>
-    <t>close add screen
-new address displayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Address is saved successfully and displayed on the top of Address Book
-displayed you paste
+    <t>cho pheps dung phim mui ten len xuong, cho phep go 1 chu de tim kiesm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.1 Address is saved successfully, close Add New Sddress screen
+4.2 New Address is displayed on the top of Address Book
 </t>
   </si>
   <si>
-    <t>cho pheps dung phim mui ten len xuong, cho phep go 1 chu de tim kiesm</t>
+    <t xml:space="preserve">4.1 Address is saved successfully, system auto trim space, close Add New Sddress screen
+4.2 New Address is displayed on the top of Address Book
+</t>
+  </si>
+  <si>
+    <t>1. Input Full name URL, SQL, HTTP GET, SQL Injection, XSS 
+2. Input valid data on all mandatory fields
+3. Click on Save button
+4. Observe Full name</t>
+  </si>
+  <si>
+    <t>4.1 Address is NOT saved successfully
+4.2 Show error message below the Full Name field: "Name should contain alphabetic and numeric
+characters"</t>
+  </si>
+  <si>
+    <t>1. Paste valid data on Full name from clipbroad 
+2. Copy text from Full name to other place</t>
+  </si>
+  <si>
+    <t>1. Full name display what you copied
+2. You can paste text copied from Full name to other place</t>
+  </si>
+  <si>
+    <t>1. Input valid data on Full name
+2. Click on X icon
+3. Observe Full name</t>
+  </si>
+  <si>
+    <t>3. Full name is blank</t>
   </si>
 </sst>
 </file>
@@ -3623,30 +3625,30 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -3659,32 +3661,59 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="17" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="63" fillId="0" borderId="3" xfId="18" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="17" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="17" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="11" borderId="0" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="0" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="63" fillId="0" borderId="3" xfId="18" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="14" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="53" fillId="0" borderId="3" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="51" fillId="0" borderId="3" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="48" fillId="0" borderId="3" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="15" fillId="8" borderId="5" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3695,35 +3724,8 @@
     <xf numFmtId="164" fontId="15" fillId="8" borderId="4" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="15" fillId="8" borderId="3" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="48" fillId="0" borderId="3" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="0" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="53" fillId="0" borderId="3" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="51" fillId="0" borderId="3" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="14" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="11" borderId="0" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="27">
@@ -4856,7 +4858,7 @@
                   <c:v>4. Address display nothing and show error message below the Address field</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>cho pheps dung phim mui ten len xuong </c:v>
+                  <c:v>cho pheps dung phim mui ten len xuong, cho phep go 1 chu de tim kiesm</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3. Show error message"Please select your Province " below the Province field</c:v>
@@ -5977,36 +5979,36 @@
       <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" customHeight="1">
-      <c r="B2" s="251" t="s">
+      <c r="B2" s="247" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="251"/>
-      <c r="D2" s="251"/>
-      <c r="E2" s="251"/>
-      <c r="F2" s="251"/>
-      <c r="G2" s="251"/>
-      <c r="H2" s="251"/>
-      <c r="I2" s="251"/>
-      <c r="J2" s="252" t="s">
+      <c r="C2" s="247"/>
+      <c r="D2" s="247"/>
+      <c r="E2" s="247"/>
+      <c r="F2" s="247"/>
+      <c r="G2" s="247"/>
+      <c r="H2" s="247"/>
+      <c r="I2" s="247"/>
+      <c r="J2" s="248" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="252"/>
+      <c r="K2" s="248"/>
     </row>
     <row r="3" spans="1:11" ht="28.5" customHeight="1">
-      <c r="B3" s="253" t="s">
+      <c r="B3" s="249" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="253"/>
-      <c r="D3" s="253"/>
-      <c r="E3" s="253"/>
-      <c r="F3" s="254" t="s">
+      <c r="C3" s="249"/>
+      <c r="D3" s="249"/>
+      <c r="E3" s="249"/>
+      <c r="F3" s="250" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="254"/>
-      <c r="H3" s="254"/>
-      <c r="I3" s="254"/>
-      <c r="J3" s="252"/>
-      <c r="K3" s="252"/>
+      <c r="G3" s="250"/>
+      <c r="H3" s="250"/>
+      <c r="I3" s="250"/>
+      <c r="J3" s="248"/>
+      <c r="K3" s="248"/>
     </row>
     <row r="4" spans="1:11" ht="18" customHeight="1">
       <c r="B4" s="26"/>
@@ -6026,65 +6028,65 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A7" s="249" t="s">
+      <c r="A7" s="251" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
-      <c r="D7" s="249"/>
-      <c r="E7" s="249"/>
-      <c r="F7" s="249"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="249"/>
-      <c r="I7" s="249"/>
+      <c r="B7" s="251"/>
+      <c r="C7" s="251"/>
+      <c r="D7" s="251"/>
+      <c r="E7" s="251"/>
+      <c r="F7" s="251"/>
+      <c r="G7" s="251"/>
+      <c r="H7" s="251"/>
+      <c r="I7" s="251"/>
     </row>
     <row r="8" spans="1:11" ht="20.25" customHeight="1">
-      <c r="A8" s="249"/>
-      <c r="B8" s="249"/>
-      <c r="C8" s="249"/>
-      <c r="D8" s="249"/>
-      <c r="E8" s="249"/>
-      <c r="F8" s="249"/>
-      <c r="G8" s="249"/>
-      <c r="H8" s="249"/>
-      <c r="I8" s="249"/>
+      <c r="A8" s="251"/>
+      <c r="B8" s="251"/>
+      <c r="C8" s="251"/>
+      <c r="D8" s="251"/>
+      <c r="E8" s="251"/>
+      <c r="F8" s="251"/>
+      <c r="G8" s="251"/>
+      <c r="H8" s="251"/>
+      <c r="I8" s="251"/>
     </row>
     <row r="9" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A9" s="249" t="s">
+      <c r="A9" s="251" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="249"/>
-      <c r="C9" s="249"/>
-      <c r="D9" s="249"/>
-      <c r="E9" s="249"/>
-      <c r="F9" s="249"/>
-      <c r="G9" s="249"/>
-      <c r="H9" s="249"/>
-      <c r="I9" s="249"/>
+      <c r="B9" s="251"/>
+      <c r="C9" s="251"/>
+      <c r="D9" s="251"/>
+      <c r="E9" s="251"/>
+      <c r="F9" s="251"/>
+      <c r="G9" s="251"/>
+      <c r="H9" s="251"/>
+      <c r="I9" s="251"/>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1">
-      <c r="A10" s="249"/>
-      <c r="B10" s="249"/>
-      <c r="C10" s="249"/>
-      <c r="D10" s="249"/>
-      <c r="E10" s="249"/>
-      <c r="F10" s="249"/>
-      <c r="G10" s="249"/>
-      <c r="H10" s="249"/>
-      <c r="I10" s="249"/>
+      <c r="A10" s="251"/>
+      <c r="B10" s="251"/>
+      <c r="C10" s="251"/>
+      <c r="D10" s="251"/>
+      <c r="E10" s="251"/>
+      <c r="F10" s="251"/>
+      <c r="G10" s="251"/>
+      <c r="H10" s="251"/>
+      <c r="I10" s="251"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="250" t="s">
+      <c r="A11" s="252" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="250"/>
-      <c r="C11" s="250"/>
-      <c r="D11" s="250"/>
-      <c r="E11" s="250"/>
-      <c r="F11" s="250"/>
-      <c r="G11" s="250"/>
-      <c r="H11" s="250"/>
-      <c r="I11" s="250"/>
+      <c r="B11" s="252"/>
+      <c r="C11" s="252"/>
+      <c r="D11" s="252"/>
+      <c r="E11" s="252"/>
+      <c r="F11" s="252"/>
+      <c r="G11" s="252"/>
+      <c r="H11" s="252"/>
+      <c r="I11" s="252"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="30"/>
@@ -6106,65 +6108,65 @@
       <c r="A14" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="247" t="s">
+      <c r="B14" s="253" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="247"/>
-      <c r="D14" s="247"/>
-      <c r="E14" s="247"/>
-      <c r="F14" s="247"/>
-      <c r="G14" s="247"/>
-      <c r="H14" s="247"/>
-      <c r="I14" s="247"/>
-      <c r="J14" s="247"/>
-      <c r="K14" s="247"/>
+      <c r="C14" s="253"/>
+      <c r="D14" s="253"/>
+      <c r="E14" s="253"/>
+      <c r="F14" s="253"/>
+      <c r="G14" s="253"/>
+      <c r="H14" s="253"/>
+      <c r="I14" s="253"/>
+      <c r="J14" s="253"/>
+      <c r="K14" s="253"/>
     </row>
     <row r="15" spans="1:11" ht="14.25" customHeight="1">
       <c r="A15" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="247" t="s">
+      <c r="B15" s="253" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="247"/>
-      <c r="D15" s="247"/>
-      <c r="E15" s="247"/>
-      <c r="F15" s="247"/>
-      <c r="G15" s="247"/>
-      <c r="H15" s="247"/>
-      <c r="I15" s="247"/>
-      <c r="J15" s="247"/>
-      <c r="K15" s="247"/>
+      <c r="C15" s="253"/>
+      <c r="D15" s="253"/>
+      <c r="E15" s="253"/>
+      <c r="F15" s="253"/>
+      <c r="G15" s="253"/>
+      <c r="H15" s="253"/>
+      <c r="I15" s="253"/>
+      <c r="J15" s="253"/>
+      <c r="K15" s="253"/>
     </row>
     <row r="16" spans="1:11" ht="14.25" customHeight="1">
       <c r="A16" s="31"/>
-      <c r="B16" s="247" t="s">
+      <c r="B16" s="253" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="247"/>
-      <c r="D16" s="247"/>
-      <c r="E16" s="247"/>
-      <c r="F16" s="247"/>
-      <c r="G16" s="247"/>
-      <c r="H16" s="247"/>
-      <c r="I16" s="247"/>
-      <c r="J16" s="247"/>
-      <c r="K16" s="247"/>
+      <c r="C16" s="253"/>
+      <c r="D16" s="253"/>
+      <c r="E16" s="253"/>
+      <c r="F16" s="253"/>
+      <c r="G16" s="253"/>
+      <c r="H16" s="253"/>
+      <c r="I16" s="253"/>
+      <c r="J16" s="253"/>
+      <c r="K16" s="253"/>
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1">
       <c r="A17" s="31"/>
-      <c r="B17" s="247" t="s">
+      <c r="B17" s="253" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="247"/>
-      <c r="D17" s="247"/>
-      <c r="E17" s="247"/>
-      <c r="F17" s="247"/>
-      <c r="G17" s="247"/>
-      <c r="H17" s="247"/>
-      <c r="I17" s="247"/>
-      <c r="J17" s="247"/>
-      <c r="K17" s="247"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="253"/>
+      <c r="J17" s="253"/>
+      <c r="K17" s="253"/>
     </row>
     <row r="19" spans="1:14" ht="23.25">
       <c r="A19" s="29" t="s">
@@ -6175,40 +6177,40 @@
       <c r="A20" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="247" t="s">
+      <c r="B20" s="253" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="247"/>
-      <c r="D20" s="247"/>
-      <c r="E20" s="247"/>
-      <c r="F20" s="247"/>
-      <c r="G20" s="247"/>
+      <c r="C20" s="253"/>
+      <c r="D20" s="253"/>
+      <c r="E20" s="253"/>
+      <c r="F20" s="253"/>
+      <c r="G20" s="253"/>
     </row>
     <row r="21" spans="1:14" ht="12.75" customHeight="1">
       <c r="A21" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="247" t="s">
+      <c r="B21" s="253" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="247"/>
-      <c r="D21" s="247"/>
-      <c r="E21" s="247"/>
-      <c r="F21" s="247"/>
-      <c r="G21" s="247"/>
+      <c r="C21" s="253"/>
+      <c r="D21" s="253"/>
+      <c r="E21" s="253"/>
+      <c r="F21" s="253"/>
+      <c r="G21" s="253"/>
     </row>
     <row r="22" spans="1:14" ht="12.75" customHeight="1">
       <c r="A22" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="247" t="s">
+      <c r="B22" s="253" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="247"/>
-      <c r="D22" s="247"/>
-      <c r="E22" s="247"/>
-      <c r="F22" s="247"/>
-      <c r="G22" s="247"/>
+      <c r="C22" s="253"/>
+      <c r="D22" s="253"/>
+      <c r="E22" s="253"/>
+      <c r="F22" s="253"/>
+      <c r="G22" s="253"/>
     </row>
     <row r="24" spans="1:14" ht="23.25">
       <c r="A24" s="29" t="s">
@@ -6267,11 +6269,11 @@
       <c r="N27" s="34"/>
     </row>
     <row r="29" spans="1:14" ht="21.75" customHeight="1">
-      <c r="B29" s="248" t="s">
+      <c r="B29" s="254" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="248"/>
-      <c r="D29" s="248"/>
+      <c r="C29" s="254"/>
+      <c r="D29" s="254"/>
     </row>
     <row r="30" spans="1:14" ht="90" customHeight="1">
       <c r="B30" s="35"/>
@@ -6294,21 +6296,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B17:K17"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="A9:I10"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="B15:K15"/>
+    <mergeCell ref="B16:K16"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="J2:K3"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="A7:I8"/>
-    <mergeCell ref="A9:I10"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="B14:K14"/>
-    <mergeCell ref="B15:K15"/>
-    <mergeCell ref="B16:K16"/>
-    <mergeCell ref="B17:K17"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -6762,8 +6764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ211"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6780,10 +6782,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="23" customFormat="1" ht="14.25">
-      <c r="A1" s="264"/>
-      <c r="B1" s="264"/>
-      <c r="C1" s="264"/>
-      <c r="D1" s="264"/>
+      <c r="A1" s="259"/>
+      <c r="B1" s="259"/>
+      <c r="C1" s="259"/>
+      <c r="D1" s="259"/>
       <c r="E1" s="25"/>
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
@@ -6793,14 +6795,14 @@
       <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:25" s="23" customFormat="1" ht="26.25">
-      <c r="A2" s="265" t="s">
+      <c r="A2" s="260" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="265"/>
-      <c r="C2" s="265"/>
-      <c r="D2" s="265"/>
+      <c r="B2" s="260"/>
+      <c r="C2" s="260"/>
+      <c r="D2" s="260"/>
       <c r="E2" s="71"/>
-      <c r="F2" s="266"/>
+      <c r="F2" s="261"/>
       <c r="G2" s="56"/>
       <c r="H2" s="56"/>
       <c r="I2" s="56"/>
@@ -6810,10 +6812,10 @@
     <row r="3" spans="1:25" s="23" customFormat="1" ht="23.25">
       <c r="A3" s="72"/>
       <c r="B3" s="73"/>
-      <c r="C3" s="267"/>
-      <c r="D3" s="267"/>
+      <c r="C3" s="262"/>
+      <c r="D3" s="262"/>
       <c r="E3" s="74"/>
-      <c r="F3" s="266"/>
+      <c r="F3" s="261"/>
       <c r="G3" s="56"/>
       <c r="H3" s="56"/>
       <c r="I3" s="56"/>
@@ -6824,9 +6826,9 @@
       <c r="A4" s="163" t="s">
         <v>196</v>
       </c>
-      <c r="B4" s="261"/>
-      <c r="C4" s="261"/>
-      <c r="D4" s="261"/>
+      <c r="B4" s="263"/>
+      <c r="C4" s="263"/>
+      <c r="D4" s="263"/>
       <c r="E4" s="164"/>
       <c r="F4" s="165"/>
       <c r="G4" s="165"/>
@@ -6841,9 +6843,9 @@
       <c r="A5" s="163" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="261"/>
-      <c r="C5" s="261"/>
-      <c r="D5" s="261"/>
+      <c r="B5" s="263"/>
+      <c r="C5" s="263"/>
+      <c r="D5" s="263"/>
       <c r="E5" s="164"/>
       <c r="F5" s="165"/>
       <c r="G5" s="165"/>
@@ -6858,9 +6860,9 @@
       <c r="A6" s="163" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="261"/>
-      <c r="C6" s="261"/>
-      <c r="D6" s="261"/>
+      <c r="B6" s="263"/>
+      <c r="C6" s="263"/>
+      <c r="D6" s="263"/>
       <c r="E6" s="164"/>
       <c r="F6" s="165"/>
       <c r="G6" s="165"/>
@@ -6872,11 +6874,11 @@
       <c r="A7" s="163" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="261" t="s">
+      <c r="B7" s="263" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="261"/>
-      <c r="D7" s="261"/>
+      <c r="C7" s="263"/>
+      <c r="D7" s="263"/>
       <c r="E7" s="164"/>
       <c r="F7" s="165"/>
       <c r="G7" s="165"/>
@@ -6889,9 +6891,9 @@
       <c r="A8" s="163" t="s">
         <v>98</v>
       </c>
-      <c r="B8" s="262"/>
-      <c r="C8" s="262"/>
-      <c r="D8" s="262"/>
+      <c r="B8" s="264"/>
+      <c r="C8" s="264"/>
+      <c r="D8" s="264"/>
       <c r="E8" s="168"/>
       <c r="F8" s="165"/>
       <c r="G8" s="169"/>
@@ -7067,11 +7069,11 @@
       <c r="D16" s="181"/>
       <c r="E16" s="181"/>
       <c r="F16" s="182"/>
-      <c r="G16" s="263" t="s">
+      <c r="G16" s="265" t="s">
         <v>99</v>
       </c>
-      <c r="H16" s="263"/>
-      <c r="I16" s="263"/>
+      <c r="H16" s="265"/>
+      <c r="I16" s="265"/>
       <c r="J16" s="183"/>
     </row>
     <row r="17" spans="1:10" s="78" customFormat="1">
@@ -7142,9 +7144,7 @@
       <c r="D20" s="201" t="s">
         <v>252</v>
       </c>
-      <c r="E20" s="201" t="s">
-        <v>405</v>
-      </c>
+      <c r="E20" s="201"/>
       <c r="F20" s="201"/>
       <c r="G20" s="193"/>
       <c r="H20" s="193"/>
@@ -7202,7 +7202,7 @@
         <v>254</v>
       </c>
       <c r="C23" s="201" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="D23" s="201" t="s">
         <v>378</v>
@@ -7214,7 +7214,7 @@
       <c r="I23" s="193"/>
       <c r="J23" s="198"/>
     </row>
-    <row r="24" spans="1:10" s="79" customFormat="1" ht="51">
+    <row r="24" spans="1:10" s="79" customFormat="1" ht="63.75">
       <c r="A24" s="193">
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
@@ -7223,10 +7223,10 @@
         <v>203</v>
       </c>
       <c r="C24" s="201" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="D24" s="201" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="E24" s="201"/>
       <c r="F24" s="202"/>
@@ -7235,7 +7235,7 @@
       <c r="I24" s="193"/>
       <c r="J24" s="198"/>
     </row>
-    <row r="25" spans="1:10" s="79" customFormat="1" ht="51">
+    <row r="25" spans="1:10" s="79" customFormat="1" ht="63.75">
       <c r="A25" s="193">
         <f t="shared" ca="1" si="0"/>
         <v>6</v>
@@ -7244,10 +7244,10 @@
         <v>223</v>
       </c>
       <c r="C25" s="201" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D25" s="201" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="E25" s="200"/>
       <c r="F25" s="202"/>
@@ -7256,7 +7256,7 @@
       <c r="I25" s="193"/>
       <c r="J25" s="198"/>
     </row>
-    <row r="26" spans="1:10" s="79" customFormat="1" ht="51">
+    <row r="26" spans="1:10" s="79" customFormat="1" ht="63.75">
       <c r="A26" s="193">
         <f t="shared" ca="1" si="0"/>
         <v>7</v>
@@ -7265,10 +7265,10 @@
         <v>204</v>
       </c>
       <c r="C26" s="201" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D26" s="201" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="E26" s="200"/>
       <c r="F26" s="202"/>
@@ -7298,7 +7298,7 @@
       <c r="I27" s="193"/>
       <c r="J27" s="198"/>
     </row>
-    <row r="28" spans="1:10" s="79" customFormat="1" ht="51">
+    <row r="28" spans="1:10" s="79" customFormat="1" ht="63.75">
       <c r="A28" s="193">
         <f t="shared" ca="1" si="0"/>
         <v>9</v>
@@ -7310,7 +7310,7 @@
         <v>380</v>
       </c>
       <c r="D28" s="201" t="s">
-        <v>381</v>
+        <v>402</v>
       </c>
       <c r="E28" s="200"/>
       <c r="F28" s="204"/>
@@ -7319,7 +7319,7 @@
       <c r="I28" s="193"/>
       <c r="J28" s="198"/>
     </row>
-    <row r="29" spans="1:10" s="79" customFormat="1" ht="51">
+    <row r="29" spans="1:10" s="79" customFormat="1" ht="63.75">
       <c r="A29" s="193">
         <f t="shared" ca="1" si="0"/>
         <v>10</v>
@@ -7328,10 +7328,10 @@
         <v>202</v>
       </c>
       <c r="C29" s="201" t="s">
-        <v>382</v>
+        <v>403</v>
       </c>
       <c r="D29" s="201" t="s">
-        <v>381</v>
+        <v>404</v>
       </c>
       <c r="E29" s="200"/>
       <c r="F29" s="204"/>
@@ -7340,7 +7340,7 @@
       <c r="I29" s="193"/>
       <c r="J29" s="198"/>
     </row>
-    <row r="30" spans="1:10" s="79" customFormat="1" ht="51">
+    <row r="30" spans="1:10" s="79" customFormat="1" ht="38.25">
       <c r="A30" s="193">
         <f t="shared" ca="1" si="0"/>
         <v>11</v>
@@ -7349,7 +7349,7 @@
         <v>221</v>
       </c>
       <c r="C30" s="193" t="s">
-        <v>383</v>
+        <v>405</v>
       </c>
       <c r="D30" s="201" t="s">
         <v>406</v>
@@ -7361,7 +7361,7 @@
       <c r="I30" s="193"/>
       <c r="J30" s="198"/>
     </row>
-    <row r="31" spans="1:10" s="79" customFormat="1" ht="63.75">
+    <row r="31" spans="1:10" s="79" customFormat="1" ht="38.25">
       <c r="A31" s="193">
         <f t="shared" ca="1" si="0"/>
         <v>12</v>
@@ -7370,10 +7370,10 @@
         <v>255</v>
       </c>
       <c r="C31" s="201" t="s">
-        <v>384</v>
+        <v>407</v>
       </c>
       <c r="D31" s="201" t="s">
-        <v>385</v>
+        <v>408</v>
       </c>
       <c r="E31" s="200"/>
       <c r="F31" s="204"/>
@@ -7429,7 +7429,7 @@
         <v>328</v>
       </c>
       <c r="D34" s="201" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="E34" s="200"/>
       <c r="F34" s="212"/>
@@ -7450,7 +7450,7 @@
         <v>329</v>
       </c>
       <c r="D35" s="201" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E35" s="201"/>
       <c r="F35" s="212"/>
@@ -7492,7 +7492,7 @@
         <v>331</v>
       </c>
       <c r="D37" s="201" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="E37" s="201"/>
       <c r="F37" s="212"/>
@@ -7692,7 +7692,7 @@
         <v>315</v>
       </c>
       <c r="D47" s="201" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E47" s="214"/>
       <c r="F47" s="215"/>
@@ -7713,7 +7713,7 @@
         <v>316</v>
       </c>
       <c r="D48" s="193" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="E48" s="216"/>
       <c r="F48" s="215"/>
@@ -7940,7 +7940,7 @@
         <v>273</v>
       </c>
       <c r="E59" s="200" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="F59" s="200"/>
       <c r="G59" s="193"/>
@@ -7960,7 +7960,7 @@
         <v>314</v>
       </c>
       <c r="D60" s="201" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="E60" s="200"/>
       <c r="F60" s="200"/>
@@ -8241,7 +8241,7 @@
         <v>50</v>
       </c>
       <c r="B74" s="199" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C74" s="201" t="s">
         <v>362</v>
@@ -8563,13 +8563,13 @@
         <v>64</v>
       </c>
       <c r="B90" s="225" t="s">
+        <v>393</v>
+      </c>
+      <c r="C90" s="225" t="s">
+        <v>395</v>
+      </c>
+      <c r="D90" s="229" t="s">
         <v>398</v>
-      </c>
-      <c r="C90" s="225" t="s">
-        <v>400</v>
-      </c>
-      <c r="D90" s="229" t="s">
-        <v>403</v>
       </c>
       <c r="E90" s="231"/>
       <c r="F90" s="210"/>
@@ -8581,13 +8581,13 @@
     <row r="91" spans="1:10" s="79" customFormat="1">
       <c r="A91" s="193"/>
       <c r="B91" s="225" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="C91" s="225" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D91" s="229" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="E91" s="240"/>
       <c r="F91" s="210"/>
@@ -8790,7 +8790,7 @@
         <v>297</v>
       </c>
       <c r="D101" s="215" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E101" s="216"/>
       <c r="F101" s="217"/>
@@ -8811,7 +8811,7 @@
         <v>298</v>
       </c>
       <c r="D102" s="215" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E102" s="239"/>
       <c r="F102" s="217"/>
@@ -9615,9 +9615,9 @@
     </row>
     <row r="163" spans="1:10" s="84" customFormat="1">
       <c r="A163" s="82"/>
-      <c r="B163" s="260"/>
-      <c r="C163" s="260"/>
-      <c r="D163" s="260"/>
+      <c r="B163" s="267"/>
+      <c r="C163" s="267"/>
+      <c r="D163" s="267"/>
       <c r="E163" s="157"/>
       <c r="F163" s="147"/>
       <c r="G163" s="148"/>
@@ -9999,9 +9999,9 @@
     </row>
     <row r="195" spans="1:10" s="84" customFormat="1" ht="14.25">
       <c r="A195" s="86"/>
-      <c r="B195" s="259"/>
-      <c r="C195" s="259"/>
-      <c r="D195" s="259"/>
+      <c r="B195" s="266"/>
+      <c r="C195" s="266"/>
+      <c r="D195" s="266"/>
       <c r="E195" s="158"/>
       <c r="F195" s="152"/>
       <c r="G195" s="153"/>
@@ -10047,9 +10047,9 @@
     </row>
     <row r="199" spans="1:10" s="84" customFormat="1" ht="14.25">
       <c r="A199" s="86"/>
-      <c r="B199" s="259"/>
-      <c r="C199" s="259"/>
-      <c r="D199" s="259"/>
+      <c r="B199" s="266"/>
+      <c r="C199" s="266"/>
+      <c r="D199" s="266"/>
       <c r="E199" s="158"/>
       <c r="F199" s="152"/>
       <c r="G199" s="153"/>
@@ -10095,9 +10095,9 @@
     </row>
     <row r="203" spans="1:10" s="84" customFormat="1" ht="14.25">
       <c r="A203" s="86"/>
-      <c r="B203" s="259"/>
-      <c r="C203" s="259"/>
-      <c r="D203" s="259"/>
+      <c r="B203" s="266"/>
+      <c r="C203" s="266"/>
+      <c r="D203" s="266"/>
       <c r="E203" s="158"/>
       <c r="F203" s="152"/>
       <c r="G203" s="153"/>
@@ -10131,9 +10131,9 @@
     </row>
     <row r="206" spans="1:10" s="84" customFormat="1" ht="14.25">
       <c r="A206" s="86"/>
-      <c r="B206" s="259"/>
-      <c r="C206" s="259"/>
-      <c r="D206" s="259"/>
+      <c r="B206" s="266"/>
+      <c r="C206" s="266"/>
+      <c r="D206" s="266"/>
       <c r="E206" s="158"/>
       <c r="F206" s="152"/>
       <c r="G206" s="153"/>
@@ -10203,21 +10203,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B206:D206"/>
+    <mergeCell ref="B163:D163"/>
+    <mergeCell ref="B195:D195"/>
+    <mergeCell ref="B199:D199"/>
+    <mergeCell ref="B203:D203"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="B206:D206"/>
-    <mergeCell ref="B163:D163"/>
-    <mergeCell ref="B195:D195"/>
-    <mergeCell ref="B199:D199"/>
-    <mergeCell ref="B203:D203"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation showDropDown="1" showErrorMessage="1" sqref="G16:I17">
@@ -10281,13 +10281,13 @@
     </row>
     <row r="2" spans="1:12" s="92" customFormat="1" ht="26.25">
       <c r="A2" s="91"/>
-      <c r="C2" s="278" t="s">
+      <c r="C2" s="268" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="278"/>
-      <c r="E2" s="278"/>
-      <c r="F2" s="278"/>
-      <c r="G2" s="278"/>
+      <c r="D2" s="268"/>
+      <c r="E2" s="268"/>
+      <c r="F2" s="268"/>
+      <c r="G2" s="268"/>
       <c r="H2" s="93" t="s">
         <v>110</v>
       </c>
@@ -10298,15 +10298,15 @@
     </row>
     <row r="3" spans="1:12" s="92" customFormat="1" ht="23.25">
       <c r="A3" s="91"/>
-      <c r="C3" s="279" t="s">
+      <c r="C3" s="269" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="279"/>
+      <c r="D3" s="269"/>
       <c r="E3" s="95"/>
-      <c r="F3" s="280" t="s">
+      <c r="F3" s="270" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="280"/>
+      <c r="G3" s="270"/>
       <c r="H3" s="94"/>
       <c r="I3" s="94"/>
       <c r="J3" s="96"/>
@@ -10331,10 +10331,10 @@
       <c r="L5" s="101"/>
     </row>
     <row r="6" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B6" s="274" t="s">
+      <c r="B6" s="271" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="274"/>
+      <c r="C6" s="271"/>
       <c r="D6" s="103"/>
       <c r="E6" s="103"/>
       <c r="F6" s="103"/>
@@ -10503,11 +10503,11 @@
       <c r="G13" s="107"/>
     </row>
     <row r="14" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B14" s="274" t="s">
+      <c r="B14" s="271" t="s">
         <v>143</v>
       </c>
-      <c r="C14" s="274"/>
-      <c r="D14" s="274"/>
+      <c r="C14" s="271"/>
+      <c r="D14" s="271"/>
       <c r="E14" s="103"/>
       <c r="F14" s="103"/>
       <c r="G14" s="104"/>
@@ -10683,11 +10683,11 @@
       <c r="G22" s="107"/>
     </row>
     <row r="23" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B23" s="274" t="s">
+      <c r="B23" s="271" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="274"/>
-      <c r="D23" s="274"/>
+      <c r="C23" s="271"/>
+      <c r="D23" s="271"/>
       <c r="E23" s="103"/>
       <c r="F23" s="103"/>
       <c r="G23" s="104"/>
@@ -10733,10 +10733,10 @@
       <c r="F26" s="109" t="s">
         <v>160</v>
       </c>
-      <c r="G26" s="277" t="s">
+      <c r="G26" s="272" t="s">
         <v>107</v>
       </c>
-      <c r="H26" s="277"/>
+      <c r="H26" s="272"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="116">
@@ -10761,8 +10761,8 @@
         <f>COUNTIFS(#REF!, "*Critical*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Critical*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G27" s="275"/>
-      <c r="H27" s="275"/>
+      <c r="G27" s="273"/>
+      <c r="H27" s="273"/>
     </row>
     <row r="28" spans="1:12" ht="20.25" customHeight="1">
       <c r="A28" s="116">
@@ -10787,8 +10787,8 @@
         <f>COUNTIFS(#REF!, "*Major*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Major*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G28" s="275"/>
-      <c r="H28" s="275"/>
+      <c r="G28" s="273"/>
+      <c r="H28" s="273"/>
     </row>
     <row r="29" spans="1:12" ht="20.25" customHeight="1">
       <c r="A29" s="116">
@@ -10813,8 +10813,8 @@
         <f>COUNTIFS(#REF!, "*Normal*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Normal*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G29" s="275"/>
-      <c r="H29" s="275"/>
+      <c r="G29" s="273"/>
+      <c r="H29" s="273"/>
     </row>
     <row r="30" spans="1:12" ht="20.25" customHeight="1">
       <c r="A30" s="116">
@@ -10839,8 +10839,8 @@
         <f>COUNTIFS(#REF!, "*Minor*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Minor*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G30" s="275"/>
-      <c r="H30" s="275"/>
+      <c r="G30" s="273"/>
+      <c r="H30" s="273"/>
     </row>
     <row r="31" spans="1:12" ht="20.25" customHeight="1">
       <c r="A31" s="116"/>
@@ -10861,8 +10861,8 @@
         <f>SUM(F27:F30)</f>
         <v>#REF!</v>
       </c>
-      <c r="G31" s="275"/>
-      <c r="H31" s="275"/>
+      <c r="G31" s="273"/>
+      <c r="H31" s="273"/>
     </row>
     <row r="32" spans="1:12" ht="20.25" customHeight="1">
       <c r="A32" s="122"/>
@@ -10900,10 +10900,10 @@
       <c r="E34" s="109" t="s">
         <v>119</v>
       </c>
-      <c r="F34" s="271" t="s">
+      <c r="F34" s="274" t="s">
         <v>122</v>
       </c>
-      <c r="G34" s="271"/>
+      <c r="G34" s="274"/>
     </row>
     <row r="35" spans="1:12" s="115" customFormat="1" ht="14.25">
       <c r="A35" s="111"/>
@@ -10919,8 +10919,8 @@
       <c r="E35" s="120" t="s">
         <v>127</v>
       </c>
-      <c r="F35" s="276"/>
-      <c r="G35" s="276"/>
+      <c r="F35" s="275"/>
+      <c r="G35" s="275"/>
       <c r="H35" s="114"/>
       <c r="I35" s="114"/>
       <c r="J35" s="114"/>
@@ -10943,8 +10943,8 @@
       <c r="E36" s="121" t="s">
         <v>133</v>
       </c>
-      <c r="F36" s="275"/>
-      <c r="G36" s="275"/>
+      <c r="F36" s="273"/>
+      <c r="G36" s="273"/>
     </row>
     <row r="37" spans="1:12" ht="20.25" customHeight="1">
       <c r="A37" s="116">
@@ -10962,8 +10962,8 @@
       <c r="E37" s="121" t="s">
         <v>133</v>
       </c>
-      <c r="F37" s="275"/>
-      <c r="G37" s="275"/>
+      <c r="F37" s="273"/>
+      <c r="G37" s="273"/>
     </row>
     <row r="38" spans="1:12" ht="20.25" customHeight="1">
       <c r="A38" s="122"/>
@@ -10976,10 +10976,10 @@
       <c r="H38" s="126"/>
     </row>
     <row r="39" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B39" s="274" t="s">
+      <c r="B39" s="271" t="s">
         <v>176</v>
       </c>
-      <c r="C39" s="274"/>
+      <c r="C39" s="271"/>
       <c r="D39" s="103"/>
       <c r="E39" s="103"/>
       <c r="F39" s="103"/>
@@ -11003,15 +11003,15 @@
       <c r="B41" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="271" t="s">
+      <c r="C41" s="274" t="s">
         <v>178</v>
       </c>
-      <c r="D41" s="271"/>
-      <c r="E41" s="271" t="s">
+      <c r="D41" s="274"/>
+      <c r="E41" s="274" t="s">
         <v>179</v>
       </c>
-      <c r="F41" s="271"/>
-      <c r="G41" s="271"/>
+      <c r="F41" s="274"/>
+      <c r="G41" s="274"/>
       <c r="H41" s="108" t="s">
         <v>180</v>
       </c>
@@ -11023,15 +11023,15 @@
       <c r="B42" s="130" t="s">
         <v>181</v>
       </c>
-      <c r="C42" s="273" t="s">
+      <c r="C42" s="276" t="s">
         <v>182</v>
       </c>
-      <c r="D42" s="273"/>
-      <c r="E42" s="273" t="s">
+      <c r="D42" s="276"/>
+      <c r="E42" s="276" t="s">
         <v>183</v>
       </c>
-      <c r="F42" s="273"/>
-      <c r="G42" s="273"/>
+      <c r="F42" s="276"/>
+      <c r="G42" s="276"/>
       <c r="H42" s="131"/>
     </row>
     <row r="43" spans="1:12" ht="34.5" customHeight="1">
@@ -11041,15 +11041,15 @@
       <c r="B43" s="130" t="s">
         <v>181</v>
       </c>
-      <c r="C43" s="273" t="s">
+      <c r="C43" s="276" t="s">
         <v>182</v>
       </c>
-      <c r="D43" s="273"/>
-      <c r="E43" s="273" t="s">
+      <c r="D43" s="276"/>
+      <c r="E43" s="276" t="s">
         <v>183</v>
       </c>
-      <c r="F43" s="273"/>
-      <c r="G43" s="273"/>
+      <c r="F43" s="276"/>
+      <c r="G43" s="276"/>
       <c r="H43" s="131"/>
     </row>
     <row r="44" spans="1:12" ht="34.5" customHeight="1">
@@ -11059,15 +11059,15 @@
       <c r="B44" s="130" t="s">
         <v>181</v>
       </c>
-      <c r="C44" s="273" t="s">
+      <c r="C44" s="276" t="s">
         <v>182</v>
       </c>
-      <c r="D44" s="273"/>
-      <c r="E44" s="273" t="s">
+      <c r="D44" s="276"/>
+      <c r="E44" s="276" t="s">
         <v>183</v>
       </c>
-      <c r="F44" s="273"/>
-      <c r="G44" s="273"/>
+      <c r="F44" s="276"/>
+      <c r="G44" s="276"/>
       <c r="H44" s="131"/>
     </row>
     <row r="45" spans="1:12">
@@ -11079,10 +11079,10 @@
       <c r="G45" s="107"/>
     </row>
     <row r="46" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B46" s="274" t="s">
+      <c r="B46" s="271" t="s">
         <v>184</v>
       </c>
-      <c r="C46" s="274"/>
+      <c r="C46" s="271"/>
       <c r="D46" s="103"/>
       <c r="E46" s="103"/>
       <c r="F46" s="103"/>
@@ -11100,25 +11100,25 @@
       <c r="G47" s="107"/>
     </row>
     <row r="48" spans="1:12" s="135" customFormat="1" ht="21" customHeight="1">
-      <c r="A48" s="269" t="s">
+      <c r="A48" s="278" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="270" t="s">
+      <c r="B48" s="279" t="s">
         <v>186</v>
       </c>
-      <c r="C48" s="271" t="s">
+      <c r="C48" s="274" t="s">
         <v>187</v>
       </c>
-      <c r="D48" s="271"/>
-      <c r="E48" s="271"/>
-      <c r="F48" s="271"/>
-      <c r="G48" s="272" t="s">
+      <c r="D48" s="274"/>
+      <c r="E48" s="274"/>
+      <c r="F48" s="274"/>
+      <c r="G48" s="280" t="s">
         <v>152</v>
       </c>
-      <c r="H48" s="272" t="s">
+      <c r="H48" s="280" t="s">
         <v>186</v>
       </c>
-      <c r="I48" s="268" t="s">
+      <c r="I48" s="277" t="s">
         <v>188</v>
       </c>
       <c r="J48" s="134"/>
@@ -11126,8 +11126,8 @@
       <c r="L48" s="134"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="269"/>
-      <c r="B49" s="270"/>
+      <c r="A49" s="278"/>
+      <c r="B49" s="279"/>
       <c r="C49" s="136" t="s">
         <v>161</v>
       </c>
@@ -11140,13 +11140,13 @@
       <c r="F49" s="137" t="s">
         <v>164</v>
       </c>
-      <c r="G49" s="272"/>
-      <c r="H49" s="272"/>
-      <c r="I49" s="268"/>
+      <c r="G49" s="280"/>
+      <c r="H49" s="280"/>
+      <c r="I49" s="277"/>
     </row>
     <row r="50" spans="1:9" ht="38.25">
-      <c r="A50" s="269"/>
-      <c r="B50" s="270"/>
+      <c r="A50" s="278"/>
+      <c r="B50" s="279"/>
       <c r="C50" s="138" t="s">
         <v>189</v>
       </c>
@@ -11258,38 +11258,38 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B46:C46"/>
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="E41:G41"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="E42:G42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <conditionalFormatting sqref="H51">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">

</xml_diff>